<commit_message>
new excel template, repair circular image display, modified email from for reset pass
</commit_message>
<xml_diff>
--- a/public/excel template/sample101.xlsx
+++ b/public/excel template/sample101.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cnm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B28F0B-B347-4238-AD5B-0FBFB10F49A9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF696D32-200B-47F3-9341-FCFAD7438A41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add" sheetId="1" r:id="rId1"/>
     <sheet name="Reassign" sheetId="2" r:id="rId2"/>
-    <sheet name="Position" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Position" sheetId="3" r:id="rId3"/>
     <sheet name="Employee" sheetId="4" r:id="rId4"/>
     <sheet name="Parent" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>First Name</t>
   </si>
@@ -74,19 +74,22 @@
     <t>Position</t>
   </si>
   <si>
-    <t>Parent Name</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
     <t>Hired Date</t>
   </si>
   <si>
-    <t>Position ID</t>
-  </si>
-  <si>
-    <t>Parent AID</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Current Parent</t>
+  </si>
+  <si>
+    <t>New Parent</t>
   </si>
   <si>
     <t>Parent Code</t>
@@ -95,18 +98,6 @@
     <t>Parent ID</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Current Parent</t>
-  </si>
-  <si>
-    <t>New Parent</t>
-  </si>
-  <si>
     <t>F.HRM M.HRM L.HRM</t>
   </si>
   <si>
@@ -152,6 +143,9 @@
     <t>F.TL1 M.TL1 L.TL1</t>
   </si>
   <si>
+    <t>F.TL2 M.TL2 L.TL2</t>
+  </si>
+  <si>
     <t>F.agent1 M.agent1 L.agent1</t>
   </si>
   <si>
@@ -203,32 +197,35 @@
     <t>agent</t>
   </si>
   <si>
-    <t>Emmanuel James</t>
-  </si>
-  <si>
-    <t>Eng</t>
-  </si>
-  <si>
-    <t>Lajom</t>
-  </si>
-  <si>
-    <t>Male</t>
+    <t>emmanuel james</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>lajom</t>
   </si>
   <si>
     <t>Davao</t>
   </si>
   <si>
-    <t>j@lajom.eng</t>
-  </si>
-  <si>
-    <t>F.TL2 M.TL2 L.TL2</t>
+    <t>jeng.lajom@yahoo.com.ph</t>
+  </si>
+  <si>
+    <t>09399999222</t>
+  </si>
+  <si>
+    <t>dsad</t>
+  </si>
+  <si>
+    <t>dsadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -239,6 +236,12 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,16 +265,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -285,53 +293,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98C783C6-4FCA-4BA4-B22F-4CBEA2494AAD}" name="Table1" displayName="Table1" ref="A1:T2" totalsRowShown="0">
-  <autoFilter ref="A1:T2" xr:uid="{329D22F9-3E70-4034-989E-48B0F1638C96}"/>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{CF2AE1DB-49DA-49FE-AD27-DE6218C9AB77}" name="First Name"/>
-    <tableColumn id="2" xr3:uid="{D42E14AA-E62B-4C58-A299-A94FB99B9B0A}" name="Middle Name"/>
-    <tableColumn id="3" xr3:uid="{17B7851C-FA66-44A9-98FA-C231E5729356}" name="Last Name"/>
-    <tableColumn id="4" xr3:uid="{DA0F4BEB-2BEE-4B10-9E92-1F03444C5231}" name="Gender"/>
-    <tableColumn id="5" xr3:uid="{C3ABB548-1FA1-473B-876F-B987928334A5}" name="Birth Date"/>
-    <tableColumn id="6" xr3:uid="{2E609E0C-BDC1-456D-B282-44904EF0D49E}" name="Address"/>
-    <tableColumn id="7" xr3:uid="{B4815994-8F0B-44F7-9E7A-FDE38D188DE5}" name="Email" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{BB9A94AD-586C-4555-8EB5-6E50B272AD60}" name="Contact No."/>
-    <tableColumn id="9" xr3:uid="{DB6BC8F2-4F77-4550-91E0-83C3BBCFB206}" name="SSS"/>
-    <tableColumn id="10" xr3:uid="{0BD04A1B-F018-468B-B397-8CE859C13E87}" name="PhilHealth"/>
-    <tableColumn id="11" xr3:uid="{3228E775-E647-43A4-92E4-6943C5F8EDE9}" name="PagIbig"/>
-    <tableColumn id="12" xr3:uid="{16E5141F-B511-44D7-8179-8A803275A9BD}" name="TIN"/>
-    <tableColumn id="13" xr3:uid="{D766DB63-6E16-4E74-B0C7-BDE35BF19EBC}" name="Position"/>
-    <tableColumn id="14" xr3:uid="{C58FF633-90F7-4BC9-9C47-917442E0C759}" name="Parent Name"/>
-    <tableColumn id="15" xr3:uid="{BB95FDC9-825A-47D3-A801-14149F3123FE}" name="Salary"/>
-    <tableColumn id="16" xr3:uid="{FA94D04D-4897-479C-907B-EAAAECA8EB25}" name="Hired Date"/>
-    <tableColumn id="17" xr3:uid="{101A23B9-D864-4804-BDE1-5932F2913ED9}" name="Position ID">
-      <calculatedColumnFormula>IF(Table1[Position]&lt;&gt;"",INDEX(Position!A:A,MATCH(Table1[Position],Position!C:C,0),0),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="18" xr3:uid="{351ED628-A5ED-4534-A63F-3BA4A2F176C0}" name="Parent AID">
-      <calculatedColumnFormula>IF(Table1[Position]&lt;&gt;"",INDEX(Position!D:D,MATCH(Table1[Position],Position!C:C,0),0),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="19" xr3:uid="{2C57EE52-BAC5-4D9E-A52A-345A899D8543}" name="Parent Code">
-      <calculatedColumnFormula>IF(Table1[Position]&lt;&gt;"",INDEX(Position!B:B,MATCH(Table1[Parent AID],Position!A:A,0),0),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="20" xr3:uid="{14C8D3FA-4F22-4D6B-8B6C-6B7F5170CD1C}" name="Parent ID">
-      <calculatedColumnFormula>IF(Table1[Parent Name]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table1[Parent Name],Employee!B:B,0),0),"")</calculatedColumnFormula>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{460D7095-ACA6-4210-A651-55655E4598AF}" name="Table1" displayName="Table1" ref="A1:O2" totalsRowShown="0">
+  <autoFilter ref="A1:O2" xr:uid="{F90B930E-AE20-462C-B19E-D674E2A1F1A4}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{1F860682-E866-44C0-AEA4-61B659F6B7C4}" name="First Name"/>
+    <tableColumn id="2" xr3:uid="{05D63B31-C6F6-46F9-9E97-DDA3BC9B9391}" name="Middle Name"/>
+    <tableColumn id="3" xr3:uid="{1091E973-8BB6-4E0C-83AB-7475278932DD}" name="Last Name"/>
+    <tableColumn id="4" xr3:uid="{C1E7C66A-05FC-4BC3-9134-5EF6BF0250D1}" name="Gender"/>
+    <tableColumn id="5" xr3:uid="{4844017C-F61E-4896-9CD1-95D6385B2142}" name="Birth Date"/>
+    <tableColumn id="6" xr3:uid="{8E635FF0-2072-4AD2-9626-5C52D7D50F3B}" name="Address"/>
+    <tableColumn id="7" xr3:uid="{476D74F7-7E1D-44EE-8013-0A709FC2EECF}" name="Email" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{A42896BD-9706-4ABB-821E-58D8AB637F07}" name="Contact No." dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{42088952-D50E-40D4-9FD4-B1C32BC99ACC}" name="SSS"/>
+    <tableColumn id="10" xr3:uid="{1B8322E0-D87D-4B57-81BA-1F0A84072634}" name="PhilHealth"/>
+    <tableColumn id="11" xr3:uid="{2507C779-8A8B-4865-A2D5-38ED6AA2B961}" name="PagIbig"/>
+    <tableColumn id="12" xr3:uid="{F8EA85B7-6399-48B1-9FA4-28CADFB9CC8B}" name="TIN"/>
+    <tableColumn id="13" xr3:uid="{9BB6ACA6-C3E3-4479-9353-29C1CDD2E177}" name="Position"/>
+    <tableColumn id="14" xr3:uid="{4C4FD9B5-0E00-4E85-AB0C-0CE9D90353EB}" name="Salary"/>
+    <tableColumn id="15" xr3:uid="{32F1FF23-E511-4BE6-9467-1600E3C55C48}" name="Hired Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF8A31D2-E6DC-4EF2-AD07-AAF7EEE1E360}" name="Table2" displayName="Table2" ref="A1:G8" totalsRowShown="0">
-  <autoFilter ref="A1:G8" xr:uid="{FF912BF4-379C-4570-B264-BD04391BBCBC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26C54B5C-A92B-4017-8645-5FCBA649D8A5}" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0">
+  <autoFilter ref="A1:G9" xr:uid="{C98DBBF9-8C25-4E91-9F18-85136F0820B2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9A6D3FCD-806B-458E-BA67-2DCF1C3F1805}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{7C2B9163-DE56-436E-AE75-AA35AB748E73}" name="Full Name"/>
-    <tableColumn id="3" xr3:uid="{D6625DAC-531F-4147-9DD9-D1B0DDEFEAF8}" name="Position"/>
-    <tableColumn id="4" xr3:uid="{AE33EBF4-AC99-448C-8609-FFA9312E412B}" name="Current Parent"/>
-    <tableColumn id="5" xr3:uid="{844490A6-A830-4E79-8D49-9DDC478DA39B}" name="New Parent"/>
-    <tableColumn id="6" xr3:uid="{B33F8848-4154-4B93-BDAA-BCCF2B1FA796}" name="Parent Code"/>
-    <tableColumn id="7" xr3:uid="{91CE72C8-CF31-490C-8A68-D3E2BE9EF88D}" name="Parent ID">
+    <tableColumn id="1" xr3:uid="{B5BFA6C1-0183-495D-BD3E-3185169DA2B3}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{505C4087-1CDB-419F-A66A-BF649E2D0D9E}" name="Full Name"/>
+    <tableColumn id="3" xr3:uid="{2E1D5EC4-1FD5-4656-A6CC-B1C8E9F52BBD}" name="Position"/>
+    <tableColumn id="4" xr3:uid="{0BA8E922-2B9C-4664-A06A-BD14723C18D6}" name="Current Parent"/>
+    <tableColumn id="5" xr3:uid="{63243E94-2768-4DCD-9516-3A6B41018AF5}" name="New Parent"/>
+    <tableColumn id="6" xr3:uid="{2BDD5A73-B150-4E2F-8486-5916266561B3}" name="Parent Code"/>
+    <tableColumn id="7" xr3:uid="{7D4C39A1-8A8D-4E94-9C23-9C9B5BB60E17}" name="Parent ID">
       <calculatedColumnFormula>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -626,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,15 +639,10 @@
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,121 +688,85 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1">
-        <v>40461</v>
-      </c>
-      <c r="F2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2">
-        <v>99999</v>
-      </c>
       <c r="I2">
-        <v>8585858</v>
+        <v>11111</v>
       </c>
       <c r="J2">
-        <v>6565656</v>
+        <v>2222</v>
       </c>
       <c r="K2">
-        <v>45454</v>
+        <v>3333</v>
       </c>
       <c r="L2">
-        <v>1010101</v>
+        <v>4444</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2">
+        <v>31</v>
+      </c>
+      <c r="N2">
         <v>400</v>
       </c>
-      <c r="P2" s="1">
-        <v>43393</v>
-      </c>
-      <c r="Q2">
-        <f>IF(Table1[Position]&lt;&gt;"",INDEX(Position!A:A,MATCH(Table1[Position],Position!C:C,0),0),"")</f>
-        <v>4</v>
-      </c>
-      <c r="R2">
-        <f>IF(Table1[Position]&lt;&gt;"",INDEX(Position!D:D,MATCH(Table1[Position],Position!C:C,0),0),"")</f>
-        <v>1</v>
-      </c>
-      <c r="S2" t="str">
-        <f>IF(Table1[Position]&lt;&gt;"",INDEX(Position!B:B,MATCH(Table1[Parent AID],Position!A:A,0),0),"")</f>
-        <v>superadmin</v>
-      </c>
-      <c r="T2">
-        <f>IF(Table1[Parent Name]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table1[Parent Name],Employee!B:B,0),0),"")</f>
-        <v>1</v>
+      <c r="O2" s="1">
+        <v>43383</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{DB594572-CB67-46E0-82EA-915BD2F962E9}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{8D873415-D0ED-4219-8EC2-1E3EA932385B}">
       <formula1>INDIRECT($M$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{18ED3460-D5A6-4DF6-B8F3-C023A5B60B8D}">
-      <formula1>INDIRECT($S2)</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{3FB37313-6AD1-4905-A10E-7AE32758B827}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{5529EDF7-3DFA-4C05-B9E7-346238A8DB70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
@@ -820,25 +774,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -846,16 +800,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
       </c>
       <c r="G2" t="str">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
@@ -867,16 +821,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" t="str">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
@@ -888,16 +842,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G4" t="str">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
@@ -909,16 +863,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G5" t="str">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
@@ -930,16 +884,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" t="str">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
@@ -951,16 +905,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G7" t="str">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
@@ -969,32 +923,53 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="str">
+        <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8">
+      <c r="G9">
         <f>IF(Table2[New Parent]&lt;&gt;"",INDEX(Employee!A:A,MATCH(Table2[New Parent],Employee!B:B,0),0),"")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8" xr:uid="{0A7C5A5F-A253-44FA-96E1-7AC7027ADCC1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{037873D1-AB76-46E5-81AA-C7F826C0431E}">
       <formula1>INDIRECT($F2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1018,10 +993,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1029,10 +1004,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1043,10 +1018,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1057,10 +1032,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1071,10 +1046,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1085,10 +1060,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1099,10 +1074,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1113,10 +1088,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1127,10 +1102,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1141,10 +1116,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1155,10 +1130,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1169,10 +1144,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -1188,9 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1199,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1210,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1221,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -1232,7 +1205,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -1243,7 +1216,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1254,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -1265,7 +1238,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1276,7 +1249,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -1287,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -1303,36 +1276,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>